<commit_message>
20250815 Real Estate x4
</commit_message>
<xml_diff>
--- a/GUI + Reviews/202506/DEUPT.xlsx
+++ b/GUI + Reviews/202506/DEUPT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://euronext-my.sharepoint.com/personal/csonneveld_euronext_com/Documents/Documents/Projects/GUI + Reviews/202506/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{90C02273-0867-472B-A424-BF15CD2E497E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4452B9A-E309-4C32-9555-8309A1C8D7D5}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{90C02273-0867-472B-A424-BF15CD2E497E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B98758FD-6E15-49A9-A387-7AB62AF64B67}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{22C33DA6-0A00-4307-AD7F-2E8886BC5899}"/>
+    <workbookView xWindow="-29115" yWindow="-16005" windowWidth="29040" windowHeight="15720" xr2:uid="{22C33DA6-0A00-4307-AD7F-2E8886BC5899}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -11739,7 +11739,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -11747,36 +11747,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="15">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -11926,6 +11920,24 @@
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -12014,22 +12026,26 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{264CD6B5-190D-484A-B540-1AE169AC6C2B}" name="Universe" displayName="Universe" ref="A1:M1284" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{5D4F82B6-CA09-4291-9E37-9482B815A8E6}" name="Name" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{08EBC2E5-8558-4165-984B-BCB5238A99AD}" name="Ticker" dataDxfId="11"/>
     <tableColumn id="3" xr3:uid="{67487B7C-C971-4725-B06A-96EAFC99E483}" name="ISIN" dataDxfId="10"/>
-    <tableColumn id="13" xr3:uid="{2D907559-A139-4232-950C-80B82FA1736E}" name="MIC" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{834C9852-DC5E-415F-9C4E-62EE948D60E8}" name="Currency (Local)" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{7C1D6969-5EBB-4398-9845-DED162666551}" name="Price (EUR) " dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{3918B1E4-5C97-49E1-B9AA-75FEF46AEFAB}" name="NOSH" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{D9B2D9C2-5D38-4E07-B0AB-B0CD1F094DA5}" name="20 days AVG turnover EUR" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{70EE6DE8-6B3D-46D9-AE18-60DB7FDDDEB2}" name="3M AVG Turnover EUR" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{B0FF23E0-B5F2-47BA-9F65-53BA5927F7C3}" name="3M AVG Turnover USD" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{9EA0C184-F582-441D-BF6E-3A55A14CB124}" name="100 Trading Days AVG Turnover EUR" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{762E6CCC-02F6-4D02-9BA9-3A557C2590B6}" name="6M AVG Turnover EUR" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{79CCBCD4-5937-4541-8D9D-E54FBC8F8155}" name="12M AVG Turnover EUR" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{2D907559-A139-4232-950C-80B82FA1736E}" name="MIC" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{834C9852-DC5E-415F-9C4E-62EE948D60E8}" name="Currency (Local)" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{7C1D6969-5EBB-4398-9845-DED162666551}" name="Price (EUR) " dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{3918B1E4-5C97-49E1-B9AA-75FEF46AEFAB}" name="NOSH" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{D9B2D9C2-5D38-4E07-B0AB-B0CD1F094DA5}" name="20 days AVG turnover EUR" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{70EE6DE8-6B3D-46D9-AE18-60DB7FDDDEB2}" name="3M AVG Turnover EUR" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{B0FF23E0-B5F2-47BA-9F65-53BA5927F7C3}" name="3M AVG Turnover USD" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{9EA0C184-F582-441D-BF6E-3A55A14CB124}" name="100 Trading Days AVG Turnover EUR" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{762E6CCC-02F6-4D02-9BA9-3A557C2590B6}" name="6M AVG Turnover EUR" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{79CCBCD4-5937-4541-8D9D-E54FBC8F8155}" name="12M AVG Turnover EUR" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -12352,10 +12368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54CB7DA4-807F-492D-BAF7-0A58E917F40F}">
-  <dimension ref="A1:M1284"/>
+  <dimension ref="A1:O1284"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A1229" workbookViewId="0">
+      <selection activeCell="G1250" sqref="G1250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -60919,7 +60935,7 @@
         <v>8303966.1565097999</v>
       </c>
     </row>
-    <row r="1185" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1185" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1185" s="1" t="s">
         <v>3566</v>
       </c>
@@ -60939,7 +60955,7 @@
         <v>78.739999999999995</v>
       </c>
       <c r="G1185" s="1">
-        <v>143188460</v>
+        <v>143188454</v>
       </c>
       <c r="H1185" s="1">
         <v>23436484.674666699</v>
@@ -60959,8 +60975,11 @@
       <c r="M1185" s="1">
         <v>24957818.781215701</v>
       </c>
-    </row>
-    <row r="1186" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O1185">
+        <v>143188460</v>
+      </c>
+    </row>
+    <row r="1186" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1186" s="1" t="s">
         <v>3569</v>
       </c>
@@ -61001,7 +61020,7 @@
         <v>9232632.4898858909</v>
       </c>
     </row>
-    <row r="1187" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1187" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1187" s="1" t="s">
         <v>3572</v>
       </c>
@@ -61042,7 +61061,7 @@
         <v>366637336.99965298</v>
       </c>
     </row>
-    <row r="1188" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1188" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1188" s="1" t="s">
         <v>3575</v>
       </c>
@@ -61083,7 +61102,7 @@
         <v>69493710.827000007</v>
       </c>
     </row>
-    <row r="1189" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1189" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1189" s="1" t="s">
         <v>3578</v>
       </c>
@@ -61124,7 +61143,7 @@
         <v>1001449.8123468501</v>
       </c>
     </row>
-    <row r="1190" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1190" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1190" s="1" t="s">
         <v>3581</v>
       </c>
@@ -61165,7 +61184,7 @@
         <v>26035722.1096825</v>
       </c>
     </row>
-    <row r="1191" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1191" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1191" s="1" t="s">
         <v>3584</v>
       </c>
@@ -61206,7 +61225,7 @@
         <v>1361235.88478261</v>
       </c>
     </row>
-    <row r="1192" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1192" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1192" s="1" t="s">
         <v>3587</v>
       </c>
@@ -61247,7 +61266,7 @@
         <v>8234061.5658891397</v>
       </c>
     </row>
-    <row r="1193" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1193" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1193" s="1" t="s">
         <v>3590</v>
       </c>
@@ -61288,7 +61307,7 @@
         <v>4401416.1344861696</v>
       </c>
     </row>
-    <row r="1194" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1194" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1194" s="1" t="s">
         <v>3593</v>
       </c>
@@ -61329,7 +61348,7 @@
         <v>17449177.935157999</v>
       </c>
     </row>
-    <row r="1195" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1195" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1195" s="1" t="s">
         <v>3596</v>
       </c>
@@ -61370,7 +61389,7 @@
         <v>32241887.72332</v>
       </c>
     </row>
-    <row r="1196" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1196" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1196" s="1" t="s">
         <v>3599</v>
       </c>
@@ -61411,7 +61430,7 @@
         <v>2841287.7557843099</v>
       </c>
     </row>
-    <row r="1197" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1197" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1197" s="1" t="s">
         <v>3602</v>
       </c>
@@ -61452,7 +61471,7 @@
         <v>962300.01884000096</v>
       </c>
     </row>
-    <row r="1198" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1198" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1198" s="1" t="s">
         <v>3605</v>
       </c>
@@ -61493,7 +61512,7 @@
         <v>12806542.978439201</v>
       </c>
     </row>
-    <row r="1199" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1199" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1199" s="1" t="s">
         <v>3608</v>
       </c>
@@ -61534,7 +61553,7 @@
         <v>2084338.59543853</v>
       </c>
     </row>
-    <row r="1200" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1200" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1200" s="1" t="s">
         <v>3611</v>
       </c>
@@ -63543,7 +63562,7 @@
         <v>2718301.0427637198</v>
       </c>
     </row>
-    <row r="1249" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1249" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1249" s="1" t="s">
         <v>3758</v>
       </c>
@@ -63563,7 +63582,7 @@
         <v>20.64</v>
       </c>
       <c r="G1249" s="1">
-        <v>231185520</v>
+        <v>231185521</v>
       </c>
       <c r="H1249" s="1">
         <v>5869381.8146666698</v>
@@ -63583,8 +63602,11 @@
       <c r="M1249" s="1">
         <v>8875219.2292745095</v>
       </c>
-    </row>
-    <row r="1250" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O1249" s="2">
+        <v>231185520</v>
+      </c>
+    </row>
+    <row r="1250" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1250" s="1" t="s">
         <v>3761</v>
       </c>
@@ -63625,7 +63647,7 @@
         <v>5026953.0633531697</v>
       </c>
     </row>
-    <row r="1251" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1251" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1251" s="1" t="s">
         <v>3764</v>
       </c>
@@ -63666,7 +63688,7 @@
         <v>12165169.265159899</v>
       </c>
     </row>
-    <row r="1252" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1252" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1252" s="1" t="s">
         <v>3767</v>
       </c>
@@ -63707,7 +63729,7 @@
         <v>3632715.4425490201</v>
       </c>
     </row>
-    <row r="1253" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1253" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1253" s="1" t="s">
         <v>3770</v>
       </c>
@@ -63748,7 +63770,7 @@
         <v>1435972.3054509801</v>
       </c>
     </row>
-    <row r="1254" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1254" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1254" s="1" t="s">
         <v>3773</v>
       </c>
@@ -63789,7 +63811,7 @@
         <v>3125551.33606649</v>
       </c>
     </row>
-    <row r="1255" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1255" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1255" s="1" t="s">
         <v>3776</v>
       </c>
@@ -63830,7 +63852,7 @@
         <v>18786306.000372499</v>
       </c>
     </row>
-    <row r="1256" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1256" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1256" s="1" t="s">
         <v>3779</v>
       </c>
@@ -63871,7 +63893,7 @@
         <v>1245446.6083618</v>
       </c>
     </row>
-    <row r="1257" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1257" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1257" s="1" t="s">
         <v>3782</v>
       </c>
@@ -63912,7 +63934,7 @@
         <v>9492074.2331225406</v>
       </c>
     </row>
-    <row r="1258" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1258" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1258" s="1" t="s">
         <v>3785</v>
       </c>
@@ -63953,7 +63975,7 @@
         <v>3322184.2613202198</v>
       </c>
     </row>
-    <row r="1259" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1259" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1259" s="1" t="s">
         <v>3788</v>
       </c>
@@ -63994,7 +64016,7 @@
         <v>827036.66848358</v>
       </c>
     </row>
-    <row r="1260" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1260" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1260" s="1" t="s">
         <v>3791</v>
       </c>
@@ -64035,7 +64057,7 @@
         <v>264419.27352717798</v>
       </c>
     </row>
-    <row r="1261" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1261" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1261" s="1" t="s">
         <v>3794</v>
       </c>
@@ -64076,7 +64098,7 @@
         <v>13198462.882495999</v>
       </c>
     </row>
-    <row r="1262" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1262" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1262" s="1" t="s">
         <v>3797</v>
       </c>
@@ -64117,7 +64139,7 @@
         <v>8383012.0861660503</v>
       </c>
     </row>
-    <row r="1263" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1263" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1263" s="1" t="s">
         <v>3800</v>
       </c>
@@ -64158,7 +64180,7 @@
         <v>78278249.928627506</v>
       </c>
     </row>
-    <row r="1264" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1264" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1264" s="1" t="s">
         <v>3803</v>
       </c>

</xml_diff>